<commit_message>
Iteration 5 der Iterationen.xlsx hinz. close #24
</commit_message>
<xml_diff>
--- a/docs/project_management/Iterationen.xlsx
+++ b/docs/project_management/Iterationen.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="108">
   <si>
     <t xml:space="preserve">Iterationsplan</t>
   </si>
@@ -222,6 +222,27 @@
   </si>
   <si>
     <t xml:space="preserve">README.md lesen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bis 18.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aktueller Stand des C4 Modell an Herrn Ringel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> möglichst alle Test Cases vollständig planen (Dokumentation/nicht Code)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11-12) alle fragen klären</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitZen etablieren, Prototyp an Si, Way of Working verfeinern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototyp übergeben</t>
   </si>
   <si>
     <t xml:space="preserve">Abgabe</t>
@@ -434,7 +455,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,6 +478,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -552,16 +577,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
@@ -999,8 +1024,87 @@
       <c r="C48" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="6" t="n">
+      <c r="D48" s="5" t="n">
         <v>44658</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="7" t="n">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="7" t="n">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" s="7" t="n">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="7" t="n">
+        <v>44669</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1129,7 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -1034,7 +1138,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -1050,132 +1154,132 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>70</v>
+      <c r="B4" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>86</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>82</v>
+        <v>88</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>91</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>74</v>
+        <v>94</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>70</v>
+        <v>97</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>38</v>
@@ -1183,13 +1287,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>74</v>
+        <v>98</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>38</v>
@@ -1197,18 +1301,18 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>70</v>
+        <v>101</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>49</v>
@@ -1216,13 +1320,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>82</v>
+        <v>103</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>19</v>
@@ -1230,13 +1334,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>82</v>
+        <v>105</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>13</v>
@@ -1244,7 +1348,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iterations ende in Iteration.xlsx angepasst
</commit_message>
<xml_diff>
--- a/docs/project_management/Iterationen.xlsx
+++ b/docs/project_management/Iterationen.xlsx
@@ -351,11 +351,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -455,7 +454,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,10 +481,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -579,11 +574,11 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.31"/>
@@ -1067,8 +1062,8 @@
       <c r="C52" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="7" t="n">
-        <v>44669</v>
+      <c r="D52" s="5" t="n">
+        <v>44676</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,8 +1073,8 @@
       <c r="C53" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="7" t="n">
-        <v>44669</v>
+      <c r="D53" s="5" t="n">
+        <v>44676</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,8 +1084,8 @@
       <c r="C54" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="7" t="n">
-        <v>44669</v>
+      <c r="D54" s="5" t="n">
+        <v>44676</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,8 +1095,8 @@
       <c r="C55" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="7" t="n">
-        <v>44669</v>
+      <c r="D55" s="5" t="n">
+        <v>44676</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>73</v>
@@ -1129,7 +1124,7 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -1161,7 +1156,7 @@
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -1175,7 +1170,7 @@
       <c r="A5" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -1186,7 +1181,7 @@
       <c r="A6" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -1200,7 +1195,7 @@
       <c r="A7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1214,7 +1209,7 @@
       <c r="A8" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -1228,7 +1223,7 @@
       <c r="A9" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1242,7 +1237,7 @@
       <c r="A10" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1261,7 +1256,7 @@
       <c r="A13" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1275,7 +1270,7 @@
       <c r="A14" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1289,7 +1284,7 @@
       <c r="A15" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -1308,7 +1303,7 @@
       <c r="A18" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -1322,7 +1317,7 @@
       <c r="A19" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -1336,7 +1331,7 @@
       <c r="A20" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C20" s="0" t="s">

</xml_diff>